<commit_message>
Changed quite a bit. Few methods added and or removed. Changed classes and added the new Layout for the GUI. Now it draws the snake and prey(this one Random). Still be changing a few things on the new GUI on the next commits.
</commit_message>
<xml_diff>
--- a/Product-backlog-template.xlsx
+++ b/Product-backlog-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jhonny\Google Drive\1 MCONTENT\UNIVERSITY\SEMESTER_1\PROGRAMMING\ASSIGNMENT_2\PROG5001A2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1B7C1A-8BCE-4195-88CB-85E83F9C8CBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040CD86F-8FE7-4A9B-8208-60001D32D54C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{49C32462-D2B8-4175-AE19-832EFB3F644D}"/>
   </bookViews>
@@ -276,7 +276,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -351,29 +351,28 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -709,40 +708,40 @@
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="35"/>
+      <c r="C1" s="40"/>
       <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="35"/>
+      <c r="C2" s="40"/>
       <c r="D2" s="27"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="35"/>
+      <c r="C3" s="40"/>
       <c r="D3" s="27"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="36"/>
+      <c r="C4" s="41"/>
       <c r="D4" s="28"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -880,11 +879,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBDA2708-75B5-4180-9C4B-08F40A18D95A}">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,7 +893,7 @@
     <col min="3" max="3" width="19.5703125" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="8" style="7" customWidth="1"/>
-    <col min="6" max="6" width="8" style="39" customWidth="1"/>
+    <col min="6" max="6" width="8" style="36" customWidth="1"/>
     <col min="7" max="7" width="8.42578125" customWidth="1"/>
     <col min="8" max="8" width="9.140625" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
@@ -997,11 +996,11 @@
       <c r="F7" s="12">
         <v>1</v>
       </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1019,11 +1018,11 @@
       <c r="F8" s="12">
         <v>1</v>
       </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1031,11 +1030,11 @@
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
@@ -1049,31 +1048,31 @@
       <c r="E10" s="8">
         <v>2</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F10" s="35">
         <f>AVERAGEA(F12:K20)</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="41">
+      <c r="A11" s="38">
         <v>3.1</v>
       </c>
       <c r="B11" s="9"/>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="39" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
@@ -1082,14 +1081,14 @@
       <c r="D12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="40">
+      <c r="F12" s="37">
         <v>0</v>
       </c>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="40"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
@@ -1099,31 +1098,31 @@
       <c r="D13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="40">
+      <c r="F13" s="37">
         <v>1</v>
       </c>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="40"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="41">
+      <c r="A14" s="38">
         <v>3.2</v>
       </c>
       <c r="B14" s="9"/>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="39" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="8"/>
-      <c r="F14" s="38"/>
+      <c r="F14" s="35"/>
       <c r="G14" s="34"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
@@ -1133,14 +1132,14 @@
       <c r="D15" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="37">
+      <c r="F15" s="34">
         <v>1</v>
       </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
@@ -1151,48 +1150,87 @@
       <c r="D16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="37">
+      <c r="F16" s="34">
         <v>0</v>
       </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="34">
+        <v>0.1</v>
+      </c>
+      <c r="H16" s="34">
+        <v>0.2</v>
+      </c>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>47</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F17" s="37">
+      <c r="F17" s="34">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="34">
+        <v>0.1</v>
+      </c>
+      <c r="H17" s="34">
+        <v>0.4</v>
+      </c>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>48</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="37">
+      <c r="F18" s="34">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="34">
+        <v>0.2</v>
+      </c>
+      <c r="H18" s="34">
+        <v>0.3</v>
+      </c>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="D19" s="4"/>
-      <c r="F19" s="37"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="34"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="D20" s="4"/>
-      <c r="F20" s="37"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>4</v>
       </c>
@@ -1206,8 +1244,20 @@
         <f>AVERAGEA(F23:F24)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="34"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>5</v>
       </c>
@@ -1220,6 +1270,291 @@
       <c r="F24" s="12">
         <v>0</v>
       </c>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="34"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="34"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="34"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="34"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="34"/>
+      <c r="K28" s="34"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="34"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="34"/>
+      <c r="K30" s="34"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="34"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="34"/>
+      <c r="J32" s="34"/>
+      <c r="K32" s="34"/>
+    </row>
+    <row r="33" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="34"/>
+    </row>
+    <row r="34" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="34"/>
+    </row>
+    <row r="35" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="34"/>
+      <c r="K35" s="34"/>
+    </row>
+    <row r="36" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G36" s="34"/>
+      <c r="H36" s="34"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
+      <c r="K36" s="34"/>
+    </row>
+    <row r="37" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G37" s="34"/>
+      <c r="H37" s="34"/>
+      <c r="I37" s="34"/>
+      <c r="J37" s="34"/>
+      <c r="K37" s="34"/>
+    </row>
+    <row r="38" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G38" s="34"/>
+      <c r="H38" s="34"/>
+      <c r="I38" s="34"/>
+      <c r="J38" s="34"/>
+      <c r="K38" s="34"/>
+    </row>
+    <row r="39" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G39" s="34"/>
+      <c r="H39" s="34"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
+      <c r="K39" s="34"/>
+    </row>
+    <row r="40" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G40" s="34"/>
+      <c r="H40" s="34"/>
+      <c r="I40" s="34"/>
+      <c r="J40" s="34"/>
+      <c r="K40" s="34"/>
+    </row>
+    <row r="41" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G41" s="34"/>
+      <c r="H41" s="34"/>
+      <c r="I41" s="34"/>
+      <c r="J41" s="34"/>
+      <c r="K41" s="34"/>
+    </row>
+    <row r="42" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G42" s="34"/>
+      <c r="H42" s="34"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
+      <c r="K42" s="34"/>
+    </row>
+    <row r="43" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G43" s="34"/>
+      <c r="H43" s="34"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
+      <c r="K43" s="34"/>
+    </row>
+    <row r="44" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G44" s="34"/>
+      <c r="H44" s="34"/>
+      <c r="I44" s="34"/>
+      <c r="J44" s="34"/>
+      <c r="K44" s="34"/>
+    </row>
+    <row r="45" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G45" s="34"/>
+      <c r="H45" s="34"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
+      <c r="K45" s="34"/>
+    </row>
+    <row r="46" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G46" s="34"/>
+      <c r="H46" s="34"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
+      <c r="K46" s="34"/>
+    </row>
+    <row r="47" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G47" s="34"/>
+      <c r="H47" s="34"/>
+      <c r="I47" s="34"/>
+      <c r="J47" s="34"/>
+      <c r="K47" s="34"/>
+    </row>
+    <row r="48" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G48" s="34"/>
+      <c r="H48" s="34"/>
+      <c r="I48" s="34"/>
+      <c r="J48" s="34"/>
+      <c r="K48" s="34"/>
+    </row>
+    <row r="49" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G49" s="34"/>
+      <c r="H49" s="34"/>
+      <c r="I49" s="34"/>
+      <c r="J49" s="34"/>
+      <c r="K49" s="34"/>
+    </row>
+    <row r="50" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G50" s="34"/>
+      <c r="H50" s="34"/>
+      <c r="I50" s="34"/>
+      <c r="J50" s="34"/>
+      <c r="K50" s="34"/>
+    </row>
+    <row r="51" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G51" s="34"/>
+      <c r="H51" s="34"/>
+      <c r="I51" s="34"/>
+      <c r="J51" s="34"/>
+      <c r="K51" s="34"/>
+    </row>
+    <row r="52" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G52" s="34"/>
+      <c r="H52" s="34"/>
+      <c r="I52" s="34"/>
+      <c r="J52" s="34"/>
+      <c r="K52" s="34"/>
+    </row>
+    <row r="53" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G53" s="34"/>
+      <c r="H53" s="34"/>
+      <c r="I53" s="34"/>
+      <c r="J53" s="34"/>
+      <c r="K53" s="34"/>
+    </row>
+    <row r="54" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G54" s="34"/>
+      <c r="H54" s="34"/>
+      <c r="I54" s="34"/>
+      <c r="J54" s="34"/>
+      <c r="K54" s="34"/>
+    </row>
+    <row r="55" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G55" s="34"/>
+      <c r="H55" s="34"/>
+      <c r="I55" s="34"/>
+      <c r="J55" s="34"/>
+      <c r="K55" s="34"/>
+    </row>
+    <row r="56" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G56" s="34"/>
+      <c r="H56" s="34"/>
+      <c r="I56" s="34"/>
+      <c r="J56" s="34"/>
+      <c r="K56" s="34"/>
+    </row>
+    <row r="57" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G57" s="34"/>
+      <c r="H57" s="34"/>
+      <c r="I57" s="34"/>
+      <c r="J57" s="34"/>
+      <c r="K57" s="34"/>
+    </row>
+    <row r="58" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G58" s="34"/>
+      <c r="H58" s="34"/>
+      <c r="I58" s="34"/>
+      <c r="J58" s="34"/>
+      <c r="K58" s="34"/>
+    </row>
+    <row r="59" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G59" s="34"/>
+      <c r="H59" s="34"/>
+      <c r="I59" s="34"/>
+      <c r="J59" s="34"/>
+      <c r="K59" s="34"/>
+    </row>
+    <row r="60" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G60" s="34"/>
+      <c r="H60" s="34"/>
+      <c r="I60" s="34"/>
+      <c r="J60" s="34"/>
+      <c r="K60" s="34"/>
+    </row>
+    <row r="61" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G61" s="34"/>
+      <c r="H61" s="34"/>
+      <c r="I61" s="34"/>
+      <c r="J61" s="34"/>
+      <c r="K61" s="34"/>
+    </row>
+    <row r="62" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G62" s="34"/>
+      <c r="H62" s="34"/>
+      <c r="I62" s="34"/>
+      <c r="J62" s="34"/>
+      <c r="K62" s="34"/>
+    </row>
+    <row r="63" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G63" s="34"/>
+      <c r="H63" s="34"/>
+      <c r="I63" s="34"/>
+      <c r="J63" s="34"/>
+      <c r="K63" s="34"/>
+    </row>
+    <row r="64" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G64" s="34"/>
+      <c r="H64" s="34"/>
+      <c r="I64" s="34"/>
+      <c r="J64" s="34"/>
+      <c r="K64" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added TopScore saving when user quits. Removed a few prints for testing, fized some bugs and updated documentation.
</commit_message>
<xml_diff>
--- a/Product-backlog-template.xlsx
+++ b/Product-backlog-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jhonny\Google Drive\1 MCONTENT\UNIVERSITY\SEMESTER_1\PROGRAMMING\ASSIGNMENT_2\PROG5001A2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040CD86F-8FE7-4A9B-8208-60001D32D54C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3577E0ED-C3F7-42D2-97BA-DF02E56A4E5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{49C32462-D2B8-4175-AE19-832EFB3F644D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t>Week 9</t>
   </si>
@@ -135,9 +135,6 @@
     <t>Owner</t>
   </si>
   <si>
-    <t>Your name and student ID</t>
-  </si>
-  <si>
     <t>Developer</t>
   </si>
   <si>
@@ -181,6 +178,24 @@
   </si>
   <si>
     <t>3.2.4</t>
+  </si>
+  <si>
+    <t>pause and resume the game by pressing the Backspace key</t>
+  </si>
+  <si>
+    <t>to see my current score based on how many preys the snake ate</t>
+  </si>
+  <si>
+    <t>I'd like to record my best score</t>
+  </si>
+  <si>
+    <t>I'd like to quit the game using a buttom</t>
+  </si>
+  <si>
+    <t>I'd like to have my top score registered even if I quite the game</t>
+  </si>
+  <si>
+    <t>Jhonathan Silva - 23605938</t>
   </si>
 </sst>
 </file>
@@ -276,7 +291,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -347,10 +362,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -367,11 +378,18 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -690,15 +708,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1F2A6E6-5A3B-4CAD-BC9F-023E52339F74}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18" style="2" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="26" style="2" customWidth="1"/>
+    <col min="3" max="3" width="3.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="78.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="2"/>
@@ -739,7 +757,7 @@
         <v>32</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C4" s="41"/>
       <c r="D4" s="28"/>
@@ -778,77 +796,99 @@
       <c r="C9" s="7">
         <v>2</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>37</v>
+      <c r="D9" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" s="7">
         <v>3</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>36</v>
+      <c r="D10" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" s="7">
         <v>4</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>40</v>
+      <c r="D11" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" s="7">
         <v>5</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>42</v>
+      <c r="D12" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C13" s="7">
         <v>6</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>38</v>
+      <c r="D13" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" s="7">
         <v>7</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>41</v>
+      <c r="D14" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" s="7">
         <v>8</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>39</v>
+      <c r="D15" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="26"/>
+      <c r="C16" s="6">
+        <v>9</v>
+      </c>
+      <c r="D16" s="42" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="33"/>
+      <c r="C17" s="38">
+        <v>10</v>
+      </c>
+      <c r="D17" s="39" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="7"/>
-      <c r="D18" s="3"/>
+      <c r="C18" s="7">
+        <v>11</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C19" s="7"/>
-      <c r="D19" s="4"/>
+      <c r="C19" s="7">
+        <v>12</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="7"/>
-      <c r="D20" s="4"/>
+      <c r="C20" s="7">
+        <v>13</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C21" s="7"/>
@@ -874,16 +914,17 @@
     <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBDA2708-75B5-4180-9C4B-08F40A18D95A}">
-  <dimension ref="A1:L64"/>
+  <dimension ref="A1:L62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,7 +934,7 @@
     <col min="3" max="3" width="19.5703125" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="8" style="7" customWidth="1"/>
-    <col min="6" max="6" width="8" style="36" customWidth="1"/>
+    <col min="6" max="6" width="8" style="34" customWidth="1"/>
     <col min="7" max="7" width="8.42578125" customWidth="1"/>
     <col min="8" max="8" width="9.140625" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
@@ -929,10 +970,10 @@
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>34</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>33</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
@@ -996,11 +1037,11 @@
       <c r="F7" s="12">
         <v>1</v>
       </c>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1018,11 +1059,11 @@
       <c r="F8" s="12">
         <v>1</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1030,11 +1071,11 @@
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
@@ -1048,31 +1089,28 @@
       <c r="E10" s="8">
         <v>2</v>
       </c>
-      <c r="F10" s="35">
-        <f>AVERAGEA(F12:K20)</f>
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="38">
+      <c r="A11" s="36">
         <v>3.1</v>
       </c>
       <c r="B11" s="9"/>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="37" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
@@ -1081,14 +1119,18 @@
       <c r="D12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="37">
+      <c r="F12" s="35">
         <v>0</v>
       </c>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32">
+        <v>0.95</v>
+      </c>
+      <c r="K12" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
@@ -1098,31 +1140,31 @@
       <c r="D13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="37">
-        <v>1</v>
-      </c>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
+      <c r="F13" s="35">
+        <v>1</v>
+      </c>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="38">
+      <c r="A14" s="36">
         <v>3.2</v>
       </c>
       <c r="B14" s="9"/>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="37" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="8"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
@@ -1130,431 +1172,433 @@
       </c>
       <c r="B15" s="5"/>
       <c r="D15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="34">
-        <v>1</v>
-      </c>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
+        <v>42</v>
+      </c>
+      <c r="F15" s="32">
+        <v>1</v>
+      </c>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="34">
+      <c r="F16" s="32">
         <v>0</v>
       </c>
-      <c r="G16" s="34">
+      <c r="G16" s="32">
         <v>0.1</v>
       </c>
-      <c r="H16" s="34">
+      <c r="H16" s="32">
         <v>0.2</v>
       </c>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
+      <c r="I16" s="32">
+        <v>0.4</v>
+      </c>
+      <c r="J16" s="32">
+        <v>1</v>
+      </c>
+      <c r="K16" s="32"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="34">
+        <v>43</v>
+      </c>
+      <c r="F17" s="32">
         <v>0</v>
       </c>
-      <c r="G17" s="34">
+      <c r="G17" s="32">
         <v>0.1</v>
       </c>
-      <c r="H17" s="34">
+      <c r="H17" s="32">
         <v>0.4</v>
       </c>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
+      <c r="I17" s="32">
+        <v>0.45</v>
+      </c>
+      <c r="J17" s="32">
+        <v>1</v>
+      </c>
+      <c r="K17" s="32"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" s="34">
+        <v>44</v>
+      </c>
+      <c r="F18" s="32">
         <v>0</v>
       </c>
-      <c r="G18" s="34">
+      <c r="G18" s="32">
         <v>0.2</v>
       </c>
-      <c r="H18" s="34">
+      <c r="H18" s="32">
         <v>0.3</v>
       </c>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="34"/>
+      <c r="I18" s="32">
+        <v>0.45</v>
+      </c>
+      <c r="J18" s="32">
+        <v>1</v>
+      </c>
+      <c r="K18" s="32"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="D19" s="4"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="D20" s="4"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
+      <c r="A20" s="8">
+        <v>4</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="8">
+        <v>3</v>
+      </c>
+      <c r="F20" s="12">
+        <v>1</v>
+      </c>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
+      <c r="G21" s="32">
+        <v>0.4</v>
+      </c>
+      <c r="H21" s="32">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="I21" s="32">
+        <v>0.76</v>
+      </c>
+      <c r="J21" s="32">
+        <v>1</v>
+      </c>
+      <c r="K21" s="32"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
+        <v>5</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="7">
         <v>4</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="8">
-        <v>3</v>
-      </c>
       <c r="F22" s="12">
-        <f>AVERAGEA(F23:F24)</f>
-        <v>0</v>
-      </c>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
+        <v>1</v>
+      </c>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32">
+        <v>1</v>
+      </c>
+      <c r="K22" s="32"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
+      <c r="K23" s="32"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
-        <v>5</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E24" s="7">
-        <v>4</v>
-      </c>
-      <c r="F24" s="12">
-        <v>0</v>
-      </c>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="34"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="34"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="34"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="34"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="32"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G29" s="34"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="34"/>
-      <c r="J29" s="34"/>
-      <c r="K29" s="34"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="32"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="34"/>
-      <c r="J30" s="34"/>
-      <c r="K30" s="34"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="32"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G31" s="34"/>
-      <c r="H31" s="34"/>
-      <c r="I31" s="34"/>
-      <c r="J31" s="34"/>
-      <c r="K31" s="34"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="32"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G32" s="34"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="34"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="34"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="32"/>
     </row>
     <row r="33" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="34"/>
-      <c r="K33" s="34"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="32"/>
     </row>
     <row r="34" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="34"/>
-      <c r="J34" s="34"/>
-      <c r="K34" s="34"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="32"/>
+      <c r="J34" s="32"/>
+      <c r="K34" s="32"/>
     </row>
     <row r="35" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G35" s="34"/>
-      <c r="H35" s="34"/>
-      <c r="I35" s="34"/>
-      <c r="J35" s="34"/>
-      <c r="K35" s="34"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="32"/>
+      <c r="J35" s="32"/>
+      <c r="K35" s="32"/>
     </row>
     <row r="36" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G36" s="34"/>
-      <c r="H36" s="34"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
-      <c r="K36" s="34"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="32"/>
     </row>
     <row r="37" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G37" s="34"/>
-      <c r="H37" s="34"/>
-      <c r="I37" s="34"/>
-      <c r="J37" s="34"/>
-      <c r="K37" s="34"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="32"/>
+      <c r="J37" s="32"/>
+      <c r="K37" s="32"/>
     </row>
     <row r="38" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G38" s="34"/>
-      <c r="H38" s="34"/>
-      <c r="I38" s="34"/>
-      <c r="J38" s="34"/>
-      <c r="K38" s="34"/>
+      <c r="G38" s="32"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="32"/>
+      <c r="J38" s="32"/>
+      <c r="K38" s="32"/>
     </row>
     <row r="39" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G39" s="34"/>
-      <c r="H39" s="34"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
-      <c r="K39" s="34"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="32"/>
+      <c r="J39" s="32"/>
+      <c r="K39" s="32"/>
     </row>
     <row r="40" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G40" s="34"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="34"/>
-      <c r="J40" s="34"/>
-      <c r="K40" s="34"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="32"/>
+      <c r="J40" s="32"/>
+      <c r="K40" s="32"/>
     </row>
     <row r="41" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G41" s="34"/>
-      <c r="H41" s="34"/>
-      <c r="I41" s="34"/>
-      <c r="J41" s="34"/>
-      <c r="K41" s="34"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="32"/>
+      <c r="I41" s="32"/>
+      <c r="J41" s="32"/>
+      <c r="K41" s="32"/>
     </row>
     <row r="42" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G42" s="34"/>
-      <c r="H42" s="34"/>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
-      <c r="K42" s="34"/>
+      <c r="G42" s="32"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="32"/>
+      <c r="J42" s="32"/>
+      <c r="K42" s="32"/>
     </row>
     <row r="43" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G43" s="34"/>
-      <c r="H43" s="34"/>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
-      <c r="K43" s="34"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="32"/>
+      <c r="J43" s="32"/>
+      <c r="K43" s="32"/>
     </row>
     <row r="44" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G44" s="34"/>
-      <c r="H44" s="34"/>
-      <c r="I44" s="34"/>
-      <c r="J44" s="34"/>
-      <c r="K44" s="34"/>
+      <c r="G44" s="32"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="32"/>
+      <c r="J44" s="32"/>
+      <c r="K44" s="32"/>
     </row>
     <row r="45" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G45" s="34"/>
-      <c r="H45" s="34"/>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
-      <c r="K45" s="34"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="32"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="32"/>
+      <c r="K45" s="32"/>
     </row>
     <row r="46" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G46" s="34"/>
-      <c r="H46" s="34"/>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
-      <c r="K46" s="34"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="32"/>
+      <c r="I46" s="32"/>
+      <c r="J46" s="32"/>
+      <c r="K46" s="32"/>
     </row>
     <row r="47" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G47" s="34"/>
-      <c r="H47" s="34"/>
-      <c r="I47" s="34"/>
-      <c r="J47" s="34"/>
-      <c r="K47" s="34"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="32"/>
+      <c r="I47" s="32"/>
+      <c r="J47" s="32"/>
+      <c r="K47" s="32"/>
     </row>
     <row r="48" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G48" s="34"/>
-      <c r="H48" s="34"/>
-      <c r="I48" s="34"/>
-      <c r="J48" s="34"/>
-      <c r="K48" s="34"/>
+      <c r="G48" s="32"/>
+      <c r="H48" s="32"/>
+      <c r="I48" s="32"/>
+      <c r="J48" s="32"/>
+      <c r="K48" s="32"/>
     </row>
     <row r="49" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G49" s="34"/>
-      <c r="H49" s="34"/>
-      <c r="I49" s="34"/>
-      <c r="J49" s="34"/>
-      <c r="K49" s="34"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
+      <c r="I49" s="32"/>
+      <c r="J49" s="32"/>
+      <c r="K49" s="32"/>
     </row>
     <row r="50" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G50" s="34"/>
-      <c r="H50" s="34"/>
-      <c r="I50" s="34"/>
-      <c r="J50" s="34"/>
-      <c r="K50" s="34"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="32"/>
+      <c r="I50" s="32"/>
+      <c r="J50" s="32"/>
+      <c r="K50" s="32"/>
     </row>
     <row r="51" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G51" s="34"/>
-      <c r="H51" s="34"/>
-      <c r="I51" s="34"/>
-      <c r="J51" s="34"/>
-      <c r="K51" s="34"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="32"/>
+      <c r="I51" s="32"/>
+      <c r="J51" s="32"/>
+      <c r="K51" s="32"/>
     </row>
     <row r="52" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G52" s="34"/>
-      <c r="H52" s="34"/>
-      <c r="I52" s="34"/>
-      <c r="J52" s="34"/>
-      <c r="K52" s="34"/>
+      <c r="G52" s="32"/>
+      <c r="H52" s="32"/>
+      <c r="I52" s="32"/>
+      <c r="J52" s="32"/>
+      <c r="K52" s="32"/>
     </row>
     <row r="53" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G53" s="34"/>
-      <c r="H53" s="34"/>
-      <c r="I53" s="34"/>
-      <c r="J53" s="34"/>
-      <c r="K53" s="34"/>
+      <c r="G53" s="32"/>
+      <c r="H53" s="32"/>
+      <c r="I53" s="32"/>
+      <c r="J53" s="32"/>
+      <c r="K53" s="32"/>
     </row>
     <row r="54" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G54" s="34"/>
-      <c r="H54" s="34"/>
-      <c r="I54" s="34"/>
-      <c r="J54" s="34"/>
-      <c r="K54" s="34"/>
+      <c r="G54" s="32"/>
+      <c r="H54" s="32"/>
+      <c r="I54" s="32"/>
+      <c r="J54" s="32"/>
+      <c r="K54" s="32"/>
     </row>
     <row r="55" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G55" s="34"/>
-      <c r="H55" s="34"/>
-      <c r="I55" s="34"/>
-      <c r="J55" s="34"/>
-      <c r="K55" s="34"/>
+      <c r="G55" s="32"/>
+      <c r="H55" s="32"/>
+      <c r="I55" s="32"/>
+      <c r="J55" s="32"/>
+      <c r="K55" s="32"/>
     </row>
     <row r="56" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G56" s="34"/>
-      <c r="H56" s="34"/>
-      <c r="I56" s="34"/>
-      <c r="J56" s="34"/>
-      <c r="K56" s="34"/>
+      <c r="G56" s="32"/>
+      <c r="H56" s="32"/>
+      <c r="I56" s="32"/>
+      <c r="J56" s="32"/>
+      <c r="K56" s="32"/>
     </row>
     <row r="57" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G57" s="34"/>
-      <c r="H57" s="34"/>
-      <c r="I57" s="34"/>
-      <c r="J57" s="34"/>
-      <c r="K57" s="34"/>
+      <c r="G57" s="32"/>
+      <c r="H57" s="32"/>
+      <c r="I57" s="32"/>
+      <c r="J57" s="32"/>
+      <c r="K57" s="32"/>
     </row>
     <row r="58" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G58" s="34"/>
-      <c r="H58" s="34"/>
-      <c r="I58" s="34"/>
-      <c r="J58" s="34"/>
-      <c r="K58" s="34"/>
+      <c r="G58" s="32"/>
+      <c r="H58" s="32"/>
+      <c r="I58" s="32"/>
+      <c r="J58" s="32"/>
+      <c r="K58" s="32"/>
     </row>
     <row r="59" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G59" s="34"/>
-      <c r="H59" s="34"/>
-      <c r="I59" s="34"/>
-      <c r="J59" s="34"/>
-      <c r="K59" s="34"/>
+      <c r="G59" s="32"/>
+      <c r="H59" s="32"/>
+      <c r="I59" s="32"/>
+      <c r="J59" s="32"/>
+      <c r="K59" s="32"/>
     </row>
     <row r="60" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G60" s="34"/>
-      <c r="H60" s="34"/>
-      <c r="I60" s="34"/>
-      <c r="J60" s="34"/>
-      <c r="K60" s="34"/>
+      <c r="G60" s="32"/>
+      <c r="H60" s="32"/>
+      <c r="I60" s="32"/>
+      <c r="J60" s="32"/>
+      <c r="K60" s="32"/>
     </row>
     <row r="61" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G61" s="34"/>
-      <c r="H61" s="34"/>
-      <c r="I61" s="34"/>
-      <c r="J61" s="34"/>
-      <c r="K61" s="34"/>
+      <c r="G61" s="32"/>
+      <c r="H61" s="32"/>
+      <c r="I61" s="32"/>
+      <c r="J61" s="32"/>
+      <c r="K61" s="32"/>
     </row>
     <row r="62" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G62" s="34"/>
-      <c r="H62" s="34"/>
-      <c r="I62" s="34"/>
-      <c r="J62" s="34"/>
-      <c r="K62" s="34"/>
-    </row>
-    <row r="63" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G63" s="34"/>
-      <c r="H63" s="34"/>
-      <c r="I63" s="34"/>
-      <c r="J63" s="34"/>
-      <c r="K63" s="34"/>
-    </row>
-    <row r="64" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G64" s="34"/>
-      <c r="H64" s="34"/>
-      <c r="I64" s="34"/>
-      <c r="J64" s="34"/>
-      <c r="K64" s="34"/>
+      <c r="G62" s="32"/>
+      <c r="H62" s="32"/>
+      <c r="I62" s="32"/>
+      <c r="J62" s="32"/>
+      <c r="K62" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>